<commit_message>
added tests for FillWavierFormSheet and fixed it (page-crossing not tested yet)
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="隊伍資料填寫" sheetId="1" state="visible" r:id="rId2"/>
@@ -1893,7 +1893,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1913,7 +1913,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="35" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="25" fillId="4" borderId="35" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2086,7 +2086,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4487,7 +4487,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.62"/>
@@ -20784,7 +20784,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.25"/>
@@ -22678,11 +22678,11 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.25"/>
@@ -24576,11 +24576,11 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.75"/>
@@ -25652,7 +25652,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37109375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="120" t="s">

</xml_diff>

<commit_message>
working base example w/ working xls & pdf conversions
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="山難留守表" sheetId="1" state="visible" r:id="rId2"/>
@@ -1078,11 +1078,11 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33984375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.25"/>
@@ -2931,8 +2931,8 @@
     <mergeCell ref="H102:I102"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.354166666666667" right="0.354166666666667" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.15" right="0" top="0.7" bottom="0.7" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2947,11 +2947,11 @@
   </sheetPr>
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33984375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.25"/>
@@ -4800,8 +4800,8 @@
     <mergeCell ref="H102:I102"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.354166666666667" right="0.354166666666667" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.15" right="0" top="0.7" bottom="0.7" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4816,11 +4816,11 @@
   </sheetPr>
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33984375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.75"/>
@@ -5872,12 +5872,15 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.354166666666667" right="0.354166666666667" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.15" right="0" top="0.7" bottom="0.7" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="40" man="true" max="16383" min="0"/>
+  </rowBreaks>
 </worksheet>
 </file>
 
@@ -5888,11 +5891,11 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33984375" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="73" t="s">
@@ -6365,7 +6368,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
fix: hotfix bug with equipment writing & fixed wavierform formatting
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="山難留守表" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,8 +15,13 @@
     <sheet name="公文用留守表_2" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="公文用留守表_3" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="切結書" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="安全守護網資料" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="切結書_2" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="安全守護網資料" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">切結書!$A$1:$J$40</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm.Print_Area" vbProcedure="false">切結書_2!$A$1:$J$40</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="74">
   <si>
     <t xml:space="preserve">台大登山社山難留守資料表 </t>
   </si>
@@ -617,7 +622,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -849,13 +854,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="double"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="double"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -882,7 +880,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1119,26 +1117,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1155,7 +1133,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1188,7 +1166,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1613,8 +1591,8 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2573,7 +2551,7 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -3317,7 +3295,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="45" zoomScaleNormal="45" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -3742,8 +3720,8 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4702,7 +4680,7 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -5444,10 +5422,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5968,458 +5946,8 @@
       <c r="I40" s="58"/>
       <c r="J40" s="41"/>
     </row>
-    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
-    </row>
-    <row r="42" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="39"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="41"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="41"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="41"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="41"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="41"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="41"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="41"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="52"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="52"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="41"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="41"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="41"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41"/>
-      <c r="B49" s="48"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="41"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="41"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="41"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="41"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="41"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="41"/>
-      <c r="B52" s="48"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="49"/>
-      <c r="G52" s="49"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="41"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="41"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="51"/>
-      <c r="J53" s="41"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="41"/>
-      <c r="B54" s="48"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="50"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="41"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="41"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="52"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="41"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="41"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="41"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="41"/>
-      <c r="B57" s="48"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="51"/>
-      <c r="J57" s="41"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="41"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="41"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="41"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="52"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="41"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="41"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="50"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="41"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="41"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="41"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="41"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="41"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="41"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="52"/>
-      <c r="I63" s="51"/>
-      <c r="J63" s="41"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="41"/>
-      <c r="B64" s="48"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="50"/>
-      <c r="I64" s="51"/>
-      <c r="J64" s="41"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="41"/>
-      <c r="B65" s="48"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="52"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="41"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="41"/>
-      <c r="B66" s="48"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="50"/>
-      <c r="I66" s="51"/>
-      <c r="J66" s="41"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="41"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="49"/>
-      <c r="D67" s="52"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="52"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="41"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="41"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="50"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="50"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="41"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="41"/>
-      <c r="B69" s="48"/>
-      <c r="C69" s="49"/>
-      <c r="D69" s="52"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="52"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="41"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="41"/>
-      <c r="B70" s="48"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="50"/>
-      <c r="E70" s="49"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="50"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="41"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="41"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="52"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="49"/>
-      <c r="G71" s="49"/>
-      <c r="H71" s="52"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="41"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="41"/>
-      <c r="B72" s="48"/>
-      <c r="C72" s="49"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="49"/>
-      <c r="F72" s="49"/>
-      <c r="G72" s="49"/>
-      <c r="H72" s="50"/>
-      <c r="I72" s="51"/>
-      <c r="J72" s="41"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="41"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="52"/>
-      <c r="E73" s="49"/>
-      <c r="F73" s="49"/>
-      <c r="G73" s="49"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="51"/>
-      <c r="J73" s="41"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="41"/>
-      <c r="B74" s="48"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="50"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="41"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="41"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="52"/>
-      <c r="E75" s="49"/>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="52"/>
-      <c r="I75" s="51"/>
-      <c r="J75" s="41"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="41"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="50"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="41"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="41"/>
-      <c r="B77" s="63"/>
-      <c r="C77" s="54"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="56"/>
-      <c r="I77" s="55"/>
-      <c r="J77" s="41"/>
-    </row>
   </sheetData>
-  <mergeCells count="216">
+  <mergeCells count="111">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="F3:I3"/>
@@ -6531,113 +6059,8 @@
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="G38:G39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="I50:I51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="I68:I69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="I72:I73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="I76:I77"/>
   </mergeCells>
-  <conditionalFormatting sqref="E6:E41 E43:E77">
+  <conditionalFormatting sqref="E6:E40">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="否" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("否",E6)))</formula>
     </cfRule>
@@ -6657,122 +6080,780 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
+  <dimension ref="A1:J40"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="2.98"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+    </row>
+    <row r="2" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="41"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="45"/>
+      <c r="J5" s="41"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="41"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="41"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="41"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="41"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="41"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="41"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="41"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="41"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="41"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="41"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="41"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="41"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="41"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="41"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="41"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="41"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="41"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="41"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="41"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="41"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="41"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="41"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="41"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="41"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="41"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="41"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="41"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="41"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="41"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="41"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="41"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="41"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="41"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="41"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="41"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="41"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="41"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="41"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="41"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="41"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="41"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="41"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="41"/>
+      <c r="B29" s="48"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="41"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="41"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="41"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="41"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="41"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="41"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="41"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="41"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="41"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="41"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="41"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="41"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="41"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="41"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="41"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="41"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="41"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="41"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="41"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="41"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="41"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="41"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="111">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="I38:I39"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E6:E40">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="否" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("否",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="66"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
     </row>
     <row r="7" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
feat: added email list of attendants
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="山難留守表" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="切結書" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="切結書_2" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="安全守護網資料" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="成員電子郵件列表" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">切結書!$A$1:$J$40</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="76">
   <si>
     <t xml:space="preserve">台大登山社山難留守資料表 </t>
   </si>
@@ -496,6 +497,12 @@
       <t xml:space="preserve">緊急聯絡人手機</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">隊員姓名</t>
+  </si>
+  <si>
+    <t xml:space="preserve">隊員信箱</t>
+  </si>
 </sst>
 </file>
 
@@ -504,7 +511,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -612,6 +619,11 @@
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="PingFang TC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -880,7 +892,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1137,6 +1149,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1577,6 +1597,41 @@
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="84.94"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5424,7 +5479,7 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test: added tests for email list & fixed some existing school ff tests
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -17,7 +17,7 @@
     <sheet name="切結書" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="切結書_2" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="安全守護網資料" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="成員電子郵件列表" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="成員Email列表" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">切結書!$A$1:$J$40</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="77">
   <si>
     <t xml:space="preserve">台大登山社山難留守資料表 </t>
   </si>
@@ -503,6 +503,9 @@
   <si>
     <t xml:space="preserve">隊員信箱</t>
   </si>
+  <si>
+    <t xml:space="preserve">成員角色</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +514,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -621,7 +624,15 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="14"/>
+      <name val="PingFang TC"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
       <name val="PingFang TC"/>
       <family val="2"/>
     </font>
@@ -1149,12 +1160,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1609,10 +1620,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1620,12 +1631,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="84.94"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>75</v>
+      </c>
+      <c r="C1" s="65" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: adjusting age requirements for waiver forms
</commit_message>
<xml_diff>
--- a/internal/dataSrc/static/source.xlsx
+++ b/internal/dataSrc/static/source.xlsx
@@ -5,19 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="山難留守表" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="山難留守表_2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="山難留守表_3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="公文用留守表" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="公文用留守表_2" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="公文用留守表_3" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="切結書" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="切結書_2" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="安全守護網資料" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="成員Email列表" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="山難留守表" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="山難留守表_2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="山難留守表_3" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="公文用留守表" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="公文用留守表_2" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="公文用留守表_3" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="切結書" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="切結書_2" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="安全守護網資料" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="成員Email列表" sheetId="10" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm.Print_Area" vbProcedure="false">切結書!$A$1:$J$40</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="78">
   <si>
     <t xml:space="preserve">台大登山社山難留守資料表 </t>
   </si>
@@ -218,7 +218,7 @@
   <si>
     <t xml:space="preserve">　　本人（簽名處見以下表格）自願報名參加由台灣大學登山社所主辦之本次活動，並聲明個人身體狀況能夠勝任此次登山活動，同時並無患有不適於登山活動的病症。
 　　在活動期間願意聽從領隊及嚮導人員之指示，並嚴謹從事，因為我清楚瞭解登山活動是有危險性的。
-　　本人為年滿二十歲之成人，若活動期間隱瞞身體狀況、不遵守領隊或隊員指導或任意嬉戲甚至私自行動導致事故發生，則事故責任自行負責，本人願意放棄一切追訴權。
+　　本人為年滿十八歲之成人，若活動期間隱瞞身體狀況、不遵守領隊或隊員指導或任意嬉戲甚至私自行動導致事故發生，則事故責任自行負責，本人願意放棄一切追訴權。
 　　立切結書人於以下： 參加人員資料  切結書簽名欄  中簽名</t>
   </si>
   <si>
@@ -249,7 +249,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">20</t>
+      <t xml:space="preserve">18</t>
     </r>
   </si>
   <si>
@@ -330,6 +330,40 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">　　本人（簽名處見以下表格）自願報名參加由台灣大學登山社所主辦之本次活動，並聲明個人身體狀況能夠勝任此次登山活動，同時並無患有不適於登山活動的病症。
+　　在活動期間願意聽從領隊及嚮導人員之指示，並嚴謹從事，因為我清楚瞭解登山活動是有危險性的。
+　　本人為年滿</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+      </rPr>
+      <t xml:space="preserve">十八</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve">歲之成人，若活動期間隱瞞身體狀況、不遵守領隊或隊員指導或任意嬉戲甚至私自行動導致事故發生，則事故責任自行負責，本人願意放棄一切追訴權。
+　　立切結書人於以下： 參加人員資料  切結書簽名欄  中簽名</t>
     </r>
   </si>
   <si>
@@ -609,6 +643,12 @@
       <charset val="136"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="22"/>
       <color rgb="FFFF0000"/>
@@ -629,12 +669,6 @@
       <name val="PingFang TC"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="PingFang TC"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -903,7 +937,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1140,11 +1174,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,11 +1194,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1190,6 +1220,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -1197,7 +1333,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1622,7 +1758,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1633,13 +1769,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="65" t="s">
         <v>76</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +1796,7 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -2620,7 +2756,7 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -3364,7 +3500,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -3789,7 +3925,7 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -4749,7 +4885,7 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -5493,8 +5629,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6151,8 +6287,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6183,7 +6319,7 @@
     </row>
     <row r="2" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -6809,7 +6945,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -6817,7 +6953,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="59"/>
       <c r="C1" s="59"/>
@@ -6830,7 +6966,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="60"/>
       <c r="C2" s="60"/>
@@ -6854,7 +6990,7 @@
     </row>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="61"/>
       <c r="C4" s="61"/>
@@ -6889,7 +7025,7 @@
     </row>
     <row r="7" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="61" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B7" s="61"/>
       <c r="C7" s="61"/>
@@ -6902,7 +7038,7 @@
     </row>
     <row r="8" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>

</xml_diff>